<commit_message>
Création BDD de test
</commit_message>
<xml_diff>
--- a/docs/data.xlsx
+++ b/docs/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\XD5965\Creative Cloud Files\01_PROJETS\01_PROG\01_APP\MyDLG\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BAF56D7-668E-4A20-9A87-A662BD6AA9EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D551485D-FAFD-4B87-A918-AE5D38867FDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8D14DDDC-9FC9-425C-962E-B3AF6E914BB2}"/>
   </bookViews>
@@ -28,7 +28,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="74">
   <si>
     <t>t_dlg</t>
   </si>
@@ -107,12 +106,6 @@
     <t>dl_zo_id</t>
   </si>
   <si>
-    <t>ex_etat</t>
-  </si>
-  <si>
-    <t>ERREUR</t>
-  </si>
-  <si>
     <t>EXPORT OK</t>
   </si>
   <si>
@@ -137,9 +130,6 @@
     <t>CRASH MAJEURE</t>
   </si>
   <si>
-    <t>CRASH MINEURE</t>
-  </si>
-  <si>
     <t>ERREURS DLG</t>
   </si>
   <si>
@@ -170,9 +160,6 @@
     <t>GO EXPORT</t>
   </si>
   <si>
-    <t>EXPORT NOK</t>
-  </si>
-  <si>
     <t>DJANGO OK</t>
   </si>
   <si>
@@ -213,13 +200,70 @@
   </si>
   <si>
     <t>PAUSE</t>
+  </si>
+  <si>
+    <t>CRASH CHECK</t>
+  </si>
+  <si>
+    <t>PE0</t>
+  </si>
+  <si>
+    <t>PE1</t>
+  </si>
+  <si>
+    <t>PE2</t>
+  </si>
+  <si>
+    <t>PE3</t>
+  </si>
+  <si>
+    <t>E0</t>
+  </si>
+  <si>
+    <t>E1</t>
+  </si>
+  <si>
+    <t>L2</t>
+  </si>
+  <si>
+    <t>A0</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>t_etats</t>
+  </si>
+  <si>
+    <t>et_id</t>
+  </si>
+  <si>
+    <t>et_code</t>
+  </si>
+  <si>
+    <t>et_nom</t>
+  </si>
+  <si>
+    <t>L0A/L0B</t>
+  </si>
+  <si>
+    <t>L1A/L1B</t>
+  </si>
+  <si>
+    <t>ex_et_code</t>
+  </si>
+  <si>
+    <t>v_dlg</t>
+  </si>
+  <si>
+    <t>v_exports_en_cours</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -240,8 +284,15 @@
       <name val="Abadi"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Abadi"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -260,8 +311,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="44">
+  <borders count="52">
     <border>
       <left/>
       <right/>
@@ -322,43 +379,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thick">
-        <color rgb="FFFF0000"/>
-      </left>
-      <right/>
-      <top style="thick">
-        <color rgb="FFFF0000"/>
-      </top>
-      <bottom style="thick">
-        <color rgb="FFFF0000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thick">
-        <color rgb="FFFF0000"/>
-      </top>
-      <bottom style="thick">
-        <color rgb="FFFF0000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thick">
-        <color rgb="FFFF0000"/>
-      </right>
-      <top style="thick">
-        <color rgb="FFFF0000"/>
-      </top>
-      <bottom style="thick">
-        <color rgb="FFFF0000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="mediumDashed">
         <color theme="1" tint="0.499984740745262"/>
       </left>
@@ -799,6 +819,171 @@
       </top>
       <bottom style="thick">
         <color rgb="FF2E76B8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF50A27D"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF50A27D"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF50A27D"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF50A27D"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="mediumDashed">
+        <color theme="1" tint="0.499984740745262"/>
+      </left>
+      <right style="mediumDashed">
+        <color theme="1" tint="0.499984740745262"/>
+      </right>
+      <top style="mediumDashed">
+        <color theme="1" tint="0.499984740745262"/>
+      </top>
+      <bottom style="mediumDashed">
+        <color theme="1" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="mediumDashed">
+        <color rgb="FF50A27D"/>
+      </left>
+      <right style="mediumDashed">
+        <color rgb="FF50A27D"/>
+      </right>
+      <top style="mediumDashed">
+        <color rgb="FF50A27D"/>
+      </top>
+      <bottom style="mediumDashed">
+        <color rgb="FF50A27D"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="mediumDashed">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right style="mediumDashed">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="mediumDashed">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom style="mediumDashed">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="mediumDashed">
+        <color rgb="FFFFC000"/>
+      </left>
+      <right style="mediumDashed">
+        <color rgb="FFFFC000"/>
+      </right>
+      <top style="mediumDashed">
+        <color rgb="FFFFC000"/>
+      </top>
+      <bottom style="mediumDashed">
+        <color rgb="FFFFC000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="mediumDashed">
+        <color rgb="FFBD8A0B"/>
+      </left>
+      <right style="mediumDashed">
+        <color rgb="FFBD8A0B"/>
+      </right>
+      <top style="mediumDashed">
+        <color rgb="FFBD8A0B"/>
+      </top>
+      <bottom style="mediumDashed">
+        <color rgb="FFBD8A0B"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF2E76B8"/>
+      </left>
+      <right style="thick">
+        <color rgb="FFC00000"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF2E76B8"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFC00000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF1EE6E1"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF760000"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF1EE6E1"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF760000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF793C94"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF793C94"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF793C94"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF793C94"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF0D0D0D"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF0D0D0D"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF0D0D0D"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF0D0D0D"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFC12975"/>
+      </left>
+      <right style="thick">
+        <color rgb="FFC12975"/>
+      </right>
+      <top style="thick">
+        <color rgb="FFC12975"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFC12975"/>
       </bottom>
       <diagonal/>
     </border>
@@ -806,7 +991,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -850,13 +1035,34 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -865,27 +1071,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -893,20 +1078,20 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -925,52 +1110,82 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -981,10 +1196,10 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF760000"/>
       <color rgb="FF0D0D0D"/>
       <color rgb="FFC12975"/>
       <color rgb="FF793C94"/>
-      <color rgb="FF760000"/>
       <color rgb="FF1EE6E1"/>
       <color rgb="FF1DDEE3"/>
       <color rgb="FF2E76B8"/>
@@ -1301,295 +1516,498 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFC023DF-5960-4085-8D7D-5FF8A6FE382A}">
-  <dimension ref="B3:I29"/>
+  <dimension ref="B2:K41"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="1"/>
-    <col min="2" max="2" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="11.42578125" style="1"/>
+    <col min="9" max="9" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B2" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B3" s="2" t="s">
-        <v>16</v>
+      <c r="B3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B4" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B5" s="1">
+      <c r="B4" s="1">
         <v>1</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C4" s="1">
         <v>24</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D4" s="1">
         <v>22</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E4" s="1">
         <v>8</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>8</v>
       </c>
     </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B6" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B7" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B8" s="2" t="s">
-        <v>0</v>
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+      <c r="D8" s="5">
+        <v>44649</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1</v>
+      </c>
+      <c r="H8" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="1">
+        <v>2</v>
+      </c>
+      <c r="C9" s="1">
         <v>1</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="3" t="s">
+      <c r="D9" s="5">
+        <v>44650</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="1">
+        <v>1</v>
+      </c>
+      <c r="H9" s="1">
         <v>2</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B10" s="1">
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B11" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" s="64" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B13" s="1">
         <v>1</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C13" s="1">
         <v>1</v>
       </c>
-      <c r="D10" s="5">
-        <v>44649</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10" s="1">
+      <c r="D13" s="1">
         <v>1</v>
       </c>
-      <c r="H10" s="1">
+      <c r="E13" s="4">
+        <v>44649.591874999998</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B14" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="D11" s="5"/>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B13" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B14" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>23</v>
+      <c r="C14" s="1">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1">
+        <v>2</v>
+      </c>
+      <c r="E14" s="4">
+        <v>44649.639062499999</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B15" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C15" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D15" s="1">
         <v>1</v>
       </c>
       <c r="E15" s="4">
-        <v>44649.591874999998</v>
+        <v>44649.691250000003</v>
       </c>
       <c r="F15" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B17" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B18" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="64" t="s">
+        <v>67</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B19" s="1">
+        <v>1</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B16" s="1">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B21" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B22" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B23" s="1">
+        <v>1</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B27" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B28" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G28" s="65" t="s">
+        <v>15</v>
+      </c>
+      <c r="H28" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="1">
+      <c r="I28" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K28" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B29" s="1">
+        <v>24</v>
+      </c>
+      <c r="C29" s="1">
+        <v>22</v>
+      </c>
+      <c r="D29" s="1">
+        <v>8</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F29" s="1">
         <v>1</v>
       </c>
-      <c r="D16" s="1">
+      <c r="G29" s="5">
+        <v>44649</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J29" s="1">
+        <v>1</v>
+      </c>
+      <c r="K29" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B30" s="1">
+        <v>24</v>
+      </c>
+      <c r="C30" s="1">
+        <v>22</v>
+      </c>
+      <c r="D30" s="1">
+        <v>8</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F30" s="1">
         <v>2</v>
       </c>
-      <c r="E16" s="4">
+      <c r="G30" s="5">
+        <v>44650</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J30" s="1">
+        <v>1</v>
+      </c>
+      <c r="K30" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="G31" s="5"/>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B32" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G32" s="5"/>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B33" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G33" s="5"/>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B34" s="1">
+        <v>1</v>
+      </c>
+      <c r="C34" s="1">
+        <v>2</v>
+      </c>
+      <c r="D34" s="4">
         <v>44649.639062499999</v>
       </c>
-      <c r="F16" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B17" s="1">
-        <v>3</v>
-      </c>
-      <c r="C17" s="1">
+      <c r="E34" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G34" s="5"/>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B35" s="1">
+        <v>2</v>
+      </c>
+      <c r="C35" s="1">
         <v>1</v>
       </c>
-      <c r="D17" s="1">
-        <v>3</v>
-      </c>
-      <c r="E17" s="4">
+      <c r="D35" s="4">
         <v>44649.691250000003</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="E35" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G35" s="5"/>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B38" s="11" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B20" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B21" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B22" s="1">
-        <v>1</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B26" s="11" t="s">
+      <c r="C38" s="11"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="11"/>
+      <c r="G38" s="11"/>
+      <c r="H38" s="11"/>
+      <c r="I38" s="11"/>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B39" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C39" s="11"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="11"/>
+      <c r="H39" s="11"/>
+      <c r="I39" s="11"/>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B40" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11"/>
-      <c r="I26" s="11"/>
-    </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B27" s="11" t="s">
+      <c r="C40" s="11"/>
+      <c r="D40" s="11"/>
+      <c r="E40" s="11"/>
+      <c r="F40" s="11"/>
+      <c r="G40" s="11"/>
+      <c r="H40" s="11"/>
+      <c r="I40" s="11"/>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B41" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C27" s="11"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="11"/>
-      <c r="I27" s="11"/>
-    </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B28" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="11"/>
-      <c r="I28" s="11"/>
-    </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B29" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="C29" s="11"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="11"/>
-      <c r="I29" s="11"/>
+      <c r="C41" s="11"/>
+      <c r="D41" s="11"/>
+      <c r="E41" s="11"/>
+      <c r="F41" s="11"/>
+      <c r="G41" s="11"/>
+      <c r="H41" s="11"/>
+      <c r="I41" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="B26:I26"/>
-    <mergeCell ref="B27:I27"/>
-    <mergeCell ref="B28:I28"/>
-    <mergeCell ref="B29:I29"/>
+    <mergeCell ref="B38:I38"/>
+    <mergeCell ref="B39:I39"/>
+    <mergeCell ref="B40:I40"/>
+    <mergeCell ref="B41:I41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1598,339 +2016,373 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24577A07-6CE2-46BC-965D-BF8C33E092FF}">
-  <dimension ref="B2:P24"/>
+  <dimension ref="B1:R23"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="1"/>
-    <col min="2" max="5" width="11.42578125" style="8"/>
-    <col min="6" max="6" width="2.85546875" style="8" customWidth="1"/>
-    <col min="7" max="10" width="11.42578125" style="8"/>
-    <col min="11" max="13" width="11.42578125" style="1"/>
-    <col min="14" max="14" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.42578125" style="1"/>
-    <col min="16" max="16" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="3.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="1"/>
+    <col min="3" max="3" width="2.85546875" style="1" customWidth="1"/>
+    <col min="4" max="7" width="11.42578125" style="8"/>
+    <col min="8" max="8" width="2.85546875" style="8" customWidth="1"/>
+    <col min="9" max="12" width="11.42578125" style="8"/>
+    <col min="13" max="15" width="11.42578125" style="1"/>
+    <col min="16" max="16" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.42578125" style="1"/>
+    <col min="18" max="18" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="2:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
-      <c r="J3" s="48"/>
-    </row>
-    <row r="4" spans="2:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-    </row>
-    <row r="5" spans="2:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="22"/>
-      <c r="J5" s="23"/>
-    </row>
-    <row r="6" spans="2:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="49"/>
-      <c r="C6" s="49"/>
-      <c r="D6" s="49"/>
-      <c r="E6" s="49"/>
-      <c r="F6" s="49"/>
-      <c r="G6" s="49"/>
-      <c r="H6" s="49"/>
-      <c r="I6" s="49"/>
-      <c r="J6" s="49"/>
-    </row>
-    <row r="7" spans="2:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="50" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" s="51"/>
-      <c r="D7" s="51"/>
-      <c r="E7" s="51"/>
-      <c r="F7" s="51"/>
-      <c r="G7" s="51"/>
-      <c r="H7" s="51"/>
-      <c r="I7" s="51"/>
-      <c r="J7" s="52"/>
-    </row>
-    <row r="8" spans="2:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="49"/>
-      <c r="C8" s="49"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="49"/>
-      <c r="F8" s="49"/>
-      <c r="G8" s="49"/>
-      <c r="H8" s="49"/>
-      <c r="I8" s="49"/>
-      <c r="J8" s="49"/>
-    </row>
-    <row r="9" spans="2:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="53" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" s="54"/>
-      <c r="D9" s="54"/>
-      <c r="E9" s="54"/>
-      <c r="F9" s="54"/>
-      <c r="G9" s="54"/>
-      <c r="H9" s="54"/>
-      <c r="I9" s="54"/>
-      <c r="J9" s="55"/>
-      <c r="N9" s="1" t="s">
+    <row r="1" spans="2:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="53" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="43" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="45"/>
+    </row>
+    <row r="3" spans="2:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+    </row>
+    <row r="4" spans="2:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="54" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="20"/>
+    </row>
+    <row r="5" spans="2:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="46"/>
+      <c r="I5" s="46"/>
+      <c r="J5" s="46"/>
+      <c r="K5" s="46"/>
+      <c r="L5" s="46"/>
+    </row>
+    <row r="6" spans="2:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="55" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" s="47" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="48"/>
+      <c r="F6" s="48"/>
+      <c r="G6" s="48"/>
+      <c r="H6" s="48"/>
+      <c r="I6" s="48"/>
+      <c r="J6" s="48"/>
+      <c r="K6" s="48"/>
+      <c r="L6" s="49"/>
+    </row>
+    <row r="7" spans="2:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D7" s="46"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="46"/>
+      <c r="J7" s="46"/>
+      <c r="K7" s="46"/>
+      <c r="L7" s="46"/>
+    </row>
+    <row r="8" spans="2:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="56" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" s="50" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" s="51"/>
+      <c r="F8" s="51"/>
+      <c r="G8" s="51"/>
+      <c r="H8" s="51"/>
+      <c r="I8" s="51"/>
+      <c r="J8" s="51"/>
+      <c r="K8" s="51"/>
+      <c r="L8" s="52"/>
+      <c r="P8" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D9" s="46"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="46"/>
+      <c r="H9" s="46"/>
+      <c r="I9" s="46"/>
+      <c r="J9" s="46"/>
+      <c r="K9" s="46"/>
+      <c r="L9" s="46"/>
+    </row>
+    <row r="10" spans="2:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="57" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="41"/>
+      <c r="J10" s="41"/>
+      <c r="K10" s="41"/>
+      <c r="L10" s="42"/>
+      <c r="P10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="R10" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="30"/>
+      <c r="K11" s="30"/>
+      <c r="L11" s="30"/>
+      <c r="P11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="R11" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="58" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="14"/>
+    </row>
+    <row r="13" spans="2:18" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+    </row>
+    <row r="14" spans="2:18" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="59" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="J14" s="22"/>
+      <c r="K14" s="22"/>
+      <c r="L14" s="23"/>
+    </row>
+    <row r="15" spans="2:18" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+    </row>
+    <row r="16" spans="2:18" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="60" t="s">
+        <v>70</v>
+      </c>
+      <c r="D16" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="J16" s="28"/>
+      <c r="K16" s="28"/>
+      <c r="L16" s="29"/>
+    </row>
+    <row r="17" spans="2:12" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30"/>
+      <c r="J17" s="30"/>
+      <c r="K17" s="30"/>
+      <c r="L17" s="30"/>
+    </row>
+    <row r="18" spans="2:12" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="61" t="s">
+        <v>62</v>
+      </c>
+      <c r="D18" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" s="32"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="32"/>
+      <c r="J18" s="32"/>
+      <c r="K18" s="32"/>
+      <c r="L18" s="33"/>
+    </row>
+    <row r="19" spans="2:12" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D19" s="30"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="30"/>
+      <c r="G19" s="30"/>
+      <c r="H19" s="30"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
+      <c r="K19" s="30"/>
+      <c r="L19" s="30"/>
+    </row>
+    <row r="20" spans="2:12" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="62" t="s">
+        <v>63</v>
+      </c>
+      <c r="D20" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="E20" s="38"/>
+      <c r="F20" s="38"/>
+      <c r="G20" s="38"/>
+      <c r="H20" s="38"/>
+      <c r="I20" s="38"/>
+      <c r="J20" s="38"/>
+      <c r="K20" s="38"/>
+      <c r="L20" s="39"/>
+    </row>
+    <row r="21" spans="2:12" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="30"/>
+      <c r="I21" s="30"/>
+      <c r="J21" s="30"/>
+      <c r="K21" s="30"/>
+      <c r="L21" s="30"/>
+    </row>
+    <row r="22" spans="2:12" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="63" t="s">
+        <v>64</v>
+      </c>
+      <c r="D22" s="34" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="10" spans="2:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="49"/>
-      <c r="C10" s="49"/>
-      <c r="D10" s="49"/>
-      <c r="E10" s="49"/>
-      <c r="F10" s="49"/>
-      <c r="G10" s="49"/>
-      <c r="H10" s="49"/>
-      <c r="I10" s="49"/>
-      <c r="J10" s="49"/>
-    </row>
-    <row r="11" spans="2:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="43" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="44"/>
-      <c r="D11" s="44"/>
-      <c r="E11" s="44"/>
-      <c r="F11" s="44"/>
-      <c r="G11" s="44"/>
-      <c r="H11" s="44"/>
-      <c r="I11" s="44"/>
-      <c r="J11" s="45"/>
-      <c r="N11" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="O11" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="P11" s="8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="12" spans="2:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="33"/>
-      <c r="C12" s="33"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="33"/>
-      <c r="G12" s="33"/>
-      <c r="H12" s="33"/>
-      <c r="I12" s="33"/>
-      <c r="J12" s="33"/>
-      <c r="N12" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="O12" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="P12" s="8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="13" spans="2:16" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="17"/>
-    </row>
-    <row r="14" spans="2:16" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-    </row>
-    <row r="15" spans="2:16" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="H15" s="25"/>
-      <c r="I15" s="25"/>
-      <c r="J15" s="26"/>
-    </row>
-    <row r="16" spans="2:16" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
-    </row>
-    <row r="17" spans="2:10" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="30" t="s">
-        <v>50</v>
-      </c>
-      <c r="H17" s="31"/>
-      <c r="I17" s="31"/>
-      <c r="J17" s="32"/>
-    </row>
-    <row r="18" spans="2:10" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="33"/>
-      <c r="C18" s="33"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="33"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
-      <c r="J18" s="33"/>
-    </row>
-    <row r="19" spans="2:10" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="C19" s="35"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="35"/>
-      <c r="F19" s="35"/>
-      <c r="G19" s="35"/>
-      <c r="H19" s="35"/>
-      <c r="I19" s="35"/>
-      <c r="J19" s="36"/>
-    </row>
-    <row r="20" spans="2:10" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="33"/>
-      <c r="C20" s="33"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="33"/>
-      <c r="F20" s="33"/>
-      <c r="G20" s="33"/>
-      <c r="H20" s="33"/>
-      <c r="I20" s="33"/>
-      <c r="J20" s="33"/>
-    </row>
-    <row r="21" spans="2:10" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="40" t="s">
-        <v>58</v>
-      </c>
-      <c r="C21" s="41"/>
-      <c r="D21" s="41"/>
-      <c r="E21" s="41"/>
-      <c r="F21" s="41"/>
-      <c r="G21" s="41"/>
-      <c r="H21" s="41"/>
-      <c r="I21" s="41"/>
-      <c r="J21" s="42"/>
-    </row>
-    <row r="22" spans="2:10" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="33"/>
-      <c r="C22" s="33"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="33"/>
-      <c r="G22" s="33"/>
-      <c r="H22" s="33"/>
-      <c r="I22" s="33"/>
-      <c r="J22" s="33"/>
-    </row>
-    <row r="23" spans="2:10" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="37" t="s">
-        <v>57</v>
-      </c>
-      <c r="C23" s="38"/>
-      <c r="D23" s="38"/>
-      <c r="E23" s="38"/>
-      <c r="F23" s="38"/>
-      <c r="G23" s="38"/>
-      <c r="H23" s="38"/>
-      <c r="I23" s="38"/>
-      <c r="J23" s="39"/>
-    </row>
-    <row r="24" spans="2:10" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="33"/>
-      <c r="C24" s="33"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="33"/>
-      <c r="G24" s="33"/>
-      <c r="H24" s="33"/>
-      <c r="I24" s="33"/>
-      <c r="J24" s="33"/>
+      <c r="E22" s="35"/>
+      <c r="F22" s="35"/>
+      <c r="G22" s="35"/>
+      <c r="H22" s="35"/>
+      <c r="I22" s="35"/>
+      <c r="J22" s="35"/>
+      <c r="K22" s="35"/>
+      <c r="L22" s="36"/>
+    </row>
+    <row r="23" spans="2:12" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="D23" s="30"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="30"/>
+      <c r="G23" s="30"/>
+      <c r="H23" s="30"/>
+      <c r="I23" s="30"/>
+      <c r="J23" s="30"/>
+      <c r="K23" s="30"/>
+      <c r="L23" s="30"/>
     </row>
   </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="B3:J3"/>
-    <mergeCell ref="B6:J6"/>
-    <mergeCell ref="B7:J7"/>
-    <mergeCell ref="B8:J8"/>
-    <mergeCell ref="B9:J9"/>
-    <mergeCell ref="B23:J23"/>
-    <mergeCell ref="B24:J24"/>
-    <mergeCell ref="B21:J21"/>
-    <mergeCell ref="B11:J11"/>
-    <mergeCell ref="B12:J12"/>
-    <mergeCell ref="B18:J18"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="G17:J17"/>
-    <mergeCell ref="B20:J20"/>
-    <mergeCell ref="B19:J19"/>
-    <mergeCell ref="B22:J22"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="B5:J5"/>
-    <mergeCell ref="G15:J15"/>
-    <mergeCell ref="B10:J10"/>
+  <mergeCells count="21">
+    <mergeCell ref="D2:L2"/>
+    <mergeCell ref="D5:L5"/>
+    <mergeCell ref="D6:L6"/>
+    <mergeCell ref="D7:L7"/>
+    <mergeCell ref="D8:L8"/>
+    <mergeCell ref="D22:L22"/>
+    <mergeCell ref="D23:L23"/>
+    <mergeCell ref="D20:L20"/>
+    <mergeCell ref="D10:L10"/>
+    <mergeCell ref="D11:L11"/>
+    <mergeCell ref="D17:L17"/>
+    <mergeCell ref="D12:L12"/>
+    <mergeCell ref="D16:G16"/>
+    <mergeCell ref="I16:L16"/>
+    <mergeCell ref="D19:L19"/>
+    <mergeCell ref="D18:L18"/>
+    <mergeCell ref="D21:L21"/>
+    <mergeCell ref="D14:G14"/>
+    <mergeCell ref="D4:L4"/>
+    <mergeCell ref="I14:L14"/>
+    <mergeCell ref="D9:L9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Construction BDD de test (requetes)
</commit_message>
<xml_diff>
--- a/docs/data.xlsx
+++ b/docs/data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\XD5965\Creative Cloud Files\01_PROJETS\01_PROG\01_APP\MyDLG\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Creative Cloud Files\01_PROJETS\01_PROG\01_APP\MyDLG\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54879C38-BFC4-4F76-9228-4D964D636CD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DCFC6FF-8030-4E95-839E-E41B6BE124FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8D14DDDC-9FC9-425C-962E-B3AF6E914BB2}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="82">
   <si>
     <t>t_dlg</t>
   </si>
@@ -163,12 +163,6 @@
     <t>DJANGO NOK</t>
   </si>
   <si>
-    <t>er_type</t>
-  </si>
-  <si>
-    <t>export/django</t>
-  </si>
-  <si>
     <t>PDB OK</t>
   </si>
   <si>
@@ -202,33 +196,6 @@
     <t>CRASH CHECK</t>
   </si>
   <si>
-    <t>PE0</t>
-  </si>
-  <si>
-    <t>PE1</t>
-  </si>
-  <si>
-    <t>PE2</t>
-  </si>
-  <si>
-    <t>PE3</t>
-  </si>
-  <si>
-    <t>E0</t>
-  </si>
-  <si>
-    <t>E1</t>
-  </si>
-  <si>
-    <t>L2</t>
-  </si>
-  <si>
-    <t>A0</t>
-  </si>
-  <si>
-    <t>A1</t>
-  </si>
-  <si>
     <t>t_etats</t>
   </si>
   <si>
@@ -241,15 +208,6 @@
     <t>et_nom</t>
   </si>
   <si>
-    <t>L0A/L0B</t>
-  </si>
-  <si>
-    <t>L1A/L1B</t>
-  </si>
-  <si>
-    <t>ex_et_code</t>
-  </si>
-  <si>
     <t>v_dlg</t>
   </si>
   <si>
@@ -257,6 +215,72 @@
   </si>
   <si>
     <t>24_NRO22_PM8_BIMI</t>
+  </si>
+  <si>
+    <t>AFA</t>
+  </si>
+  <si>
+    <t>CMA</t>
+  </si>
+  <si>
+    <t>GEX</t>
+  </si>
+  <si>
+    <t>CCH</t>
+  </si>
+  <si>
+    <t>EDL</t>
+  </si>
+  <si>
+    <t>EOK</t>
+  </si>
+  <si>
+    <t>DOK/DNO</t>
+  </si>
+  <si>
+    <t>POK/PNO</t>
+  </si>
+  <si>
+    <t>LCL</t>
+  </si>
+  <si>
+    <t>PAU</t>
+  </si>
+  <si>
+    <t>ANN</t>
+  </si>
+  <si>
+    <t>ex_et_id</t>
+  </si>
+  <si>
+    <t>1_AFA</t>
+  </si>
+  <si>
+    <t>2_CMA</t>
+  </si>
+  <si>
+    <t>ex_et_nom</t>
+  </si>
+  <si>
+    <t>ex_et_ref</t>
+  </si>
+  <si>
+    <t>t_types_erreurs</t>
+  </si>
+  <si>
+    <t>te_id</t>
+  </si>
+  <si>
+    <t>te_nom</t>
+  </si>
+  <si>
+    <t>er_te_id</t>
+  </si>
+  <si>
+    <t>export</t>
+  </si>
+  <si>
+    <t>django</t>
   </si>
 </sst>
 </file>
@@ -292,7 +316,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -317,6 +341,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="52">
     <border>
@@ -991,7 +1021,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1023,66 +1053,135 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1092,100 +1191,34 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1519,23 +1552,23 @@
   <dimension ref="B2:O35"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="24.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="19.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="20.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="20.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
@@ -1544,7 +1577,7 @@
         <v>15</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.3">
@@ -1563,14 +1596,14 @@
       <c r="F3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="K3" s="64" t="s">
-        <v>66</v>
+      <c r="J3" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>55</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.3">
@@ -1593,7 +1626,7 @@
         <v>1</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>23</v>
@@ -1604,7 +1637,7 @@
         <v>0</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>31</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.3">
@@ -1629,23 +1662,11 @@
       <c r="H7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="J7" s="3" t="s">
-        <v>32</v>
+      <c r="J7" s="66" t="s">
+        <v>77</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="M7" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="N7" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="O7" s="3" t="s">
-        <v>38</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.3">
@@ -1674,19 +1695,7 @@
         <v>1</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="O8" s="1" t="s">
-        <v>35</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.3">
@@ -1711,11 +1720,20 @@
       <c r="H9" s="1">
         <v>2</v>
       </c>
+      <c r="J9" s="1">
+        <v>2</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="J11" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
@@ -1730,8 +1748,26 @@
       <c r="E12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="64" t="s">
-        <v>70</v>
+      <c r="F12" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K12" s="66" t="s">
+        <v>79</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="O12" s="3" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.3">
@@ -1747,8 +1783,26 @@
       <c r="E13" s="4">
         <v>44649.591874999998</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>55</v>
+      <c r="F13" s="1">
+        <v>1</v>
+      </c>
+      <c r="J13" s="1">
+        <v>1</v>
+      </c>
+      <c r="K13" s="1">
+        <v>1</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.3">
@@ -1764,8 +1818,8 @@
       <c r="E14" s="4">
         <v>44649.639062499999</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>57</v>
+      <c r="F14" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.3">
@@ -1781,13 +1835,13 @@
       <c r="E15" s="4">
         <v>44649.691250000003</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>55</v>
+      <c r="F15" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B20" s="2" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.3">
@@ -1809,7 +1863,7 @@
       <c r="G21" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="H21" s="65" t="s">
+      <c r="H21" s="23" t="s">
         <v>14</v>
       </c>
       <c r="I21" s="3" t="s">
@@ -1839,7 +1893,7 @@
         <v>7</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="G22" s="1">
         <v>1</v>
@@ -1874,7 +1928,7 @@
         <v>7</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="G23" s="1">
         <v>2</v>
@@ -1900,7 +1954,7 @@
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B25" s="2" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="G25" s="5"/>
     </row>
@@ -1915,9 +1969,11 @@
         <v>12</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="G26" s="5"/>
+        <v>75</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B27" s="1">
@@ -1930,9 +1986,11 @@
         <v>44649.639062499999</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="G27" s="5"/>
+        <v>72</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B28" s="1">
@@ -1945,57 +2003,59 @@
         <v>44649.691250000003</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G28" s="5"/>
+        <v>73</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B32" s="11" t="s">
+      <c r="B32" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="C32" s="11"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11"/>
-      <c r="F32" s="11"/>
-      <c r="G32" s="11"/>
-      <c r="H32" s="11"/>
-      <c r="I32" s="11"/>
+      <c r="C32" s="24"/>
+      <c r="D32" s="24"/>
+      <c r="E32" s="24"/>
+      <c r="F32" s="24"/>
+      <c r="G32" s="24"/>
+      <c r="H32" s="24"/>
+      <c r="I32" s="24"/>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B33" s="11" t="s">
+      <c r="B33" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="C33" s="11"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="11"/>
-      <c r="F33" s="11"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="11"/>
-      <c r="I33" s="11"/>
+      <c r="C33" s="24"/>
+      <c r="D33" s="24"/>
+      <c r="E33" s="24"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="24"/>
+      <c r="H33" s="24"/>
+      <c r="I33" s="24"/>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B34" s="11" t="s">
+      <c r="B34" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="C34" s="11"/>
-      <c r="D34" s="11"/>
-      <c r="E34" s="11"/>
-      <c r="F34" s="11"/>
-      <c r="G34" s="11"/>
-      <c r="H34" s="11"/>
-      <c r="I34" s="11"/>
+      <c r="C34" s="24"/>
+      <c r="D34" s="24"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="24"/>
+      <c r="H34" s="24"/>
+      <c r="I34" s="24"/>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B35" s="11" t="s">
+      <c r="B35" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="C35" s="11"/>
-      <c r="D35" s="11"/>
-      <c r="E35" s="11"/>
-      <c r="F35" s="11"/>
-      <c r="G35" s="11"/>
-      <c r="H35" s="11"/>
-      <c r="I35" s="11"/>
+      <c r="C35" s="24"/>
+      <c r="D35" s="24"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="24"/>
+      <c r="G35" s="24"/>
+      <c r="H35" s="24"/>
+      <c r="I35" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2013,14 +2073,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24577A07-6CE2-46BC-965D-BF8C33E092FF}">
   <dimension ref="B1:R23"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="1"/>
+    <col min="2" max="2" width="13" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="2.85546875" style="1" customWidth="1"/>
     <col min="4" max="7" width="11.42578125" style="8"/>
     <col min="8" max="8" width="2.85546875" style="8" customWidth="1"/>
@@ -2034,20 +2092,20 @@
   <sheetData>
     <row r="1" spans="2:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="53" t="s">
-        <v>55</v>
-      </c>
-      <c r="D2" s="43" t="s">
+      <c r="B2" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44"/>
-      <c r="K2" s="44"/>
-      <c r="L2" s="45"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="27"/>
     </row>
     <row r="3" spans="2:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D3" s="9"/>
@@ -2061,149 +2119,149 @@
       <c r="L3" s="9"/>
     </row>
     <row r="4" spans="2:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="54" t="s">
-        <v>56</v>
-      </c>
-      <c r="D4" s="18" t="s">
+      <c r="B4" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4" s="60" t="s">
         <v>39</v>
       </c>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="19"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="20"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="61"/>
+      <c r="H4" s="61"/>
+      <c r="I4" s="61"/>
+      <c r="J4" s="61"/>
+      <c r="K4" s="61"/>
+      <c r="L4" s="62"/>
     </row>
     <row r="5" spans="2:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
-      <c r="I5" s="46"/>
-      <c r="J5" s="46"/>
-      <c r="K5" s="46"/>
-      <c r="L5" s="46"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="28"/>
+      <c r="J5" s="28"/>
+      <c r="K5" s="28"/>
+      <c r="L5" s="28"/>
     </row>
     <row r="6" spans="2:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="55" t="s">
-        <v>57</v>
-      </c>
-      <c r="D6" s="47" t="s">
+      <c r="B6" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="48"/>
-      <c r="F6" s="48"/>
-      <c r="G6" s="48"/>
-      <c r="H6" s="48"/>
-      <c r="I6" s="48"/>
-      <c r="J6" s="48"/>
-      <c r="K6" s="48"/>
-      <c r="L6" s="49"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="30"/>
+      <c r="K6" s="30"/>
+      <c r="L6" s="31"/>
     </row>
     <row r="7" spans="2:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="46"/>
-      <c r="I7" s="46"/>
-      <c r="J7" s="46"/>
-      <c r="K7" s="46"/>
-      <c r="L7" s="46"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="28"/>
+      <c r="L7" s="28"/>
     </row>
     <row r="8" spans="2:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="56" t="s">
-        <v>58</v>
-      </c>
-      <c r="D8" s="50" t="s">
-        <v>54</v>
-      </c>
-      <c r="E8" s="51"/>
-      <c r="F8" s="51"/>
-      <c r="G8" s="51"/>
-      <c r="H8" s="51"/>
-      <c r="I8" s="51"/>
-      <c r="J8" s="51"/>
-      <c r="K8" s="51"/>
-      <c r="L8" s="52"/>
+      <c r="B8" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="33"/>
+      <c r="K8" s="33"/>
+      <c r="L8" s="34"/>
       <c r="P8" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="28"/>
+    </row>
+    <row r="10" spans="2:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="42" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="43"/>
+      <c r="H10" s="43"/>
+      <c r="I10" s="43"/>
+      <c r="J10" s="43"/>
+      <c r="K10" s="43"/>
+      <c r="L10" s="44"/>
+      <c r="P10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q10" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="9" spans="2:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
-      <c r="F9" s="46"/>
-      <c r="G9" s="46"/>
-      <c r="H9" s="46"/>
-      <c r="I9" s="46"/>
-      <c r="J9" s="46"/>
-      <c r="K9" s="46"/>
-      <c r="L9" s="46"/>
-    </row>
-    <row r="10" spans="2:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="57" t="s">
-        <v>59</v>
-      </c>
-      <c r="D10" s="40" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
-      <c r="G10" s="41"/>
-      <c r="H10" s="41"/>
-      <c r="I10" s="41"/>
-      <c r="J10" s="41"/>
-      <c r="K10" s="41"/>
-      <c r="L10" s="42"/>
-      <c r="P10" s="1" t="s">
+      <c r="R10" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="Q10" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="R10" s="8" t="s">
+    </row>
+    <row r="11" spans="2:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="38"/>
+      <c r="J11" s="38"/>
+      <c r="K11" s="38"/>
+      <c r="L11" s="38"/>
+      <c r="P11" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="11" spans="2:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D11" s="30"/>
-      <c r="E11" s="30"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="30"/>
-      <c r="H11" s="30"/>
-      <c r="I11" s="30"/>
-      <c r="J11" s="30"/>
-      <c r="K11" s="30"/>
-      <c r="L11" s="30"/>
-      <c r="P11" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="Q11" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="R11" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="2:18" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="58" t="s">
-        <v>60</v>
-      </c>
-      <c r="D12" s="12" t="s">
+      <c r="B12" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="14"/>
+      <c r="E12" s="46"/>
+      <c r="F12" s="46"/>
+      <c r="G12" s="46"/>
+      <c r="H12" s="46"/>
+      <c r="I12" s="46"/>
+      <c r="J12" s="46"/>
+      <c r="K12" s="46"/>
+      <c r="L12" s="47"/>
     </row>
     <row r="13" spans="2:18" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D13" s="10"/>
@@ -2217,22 +2275,22 @@
       <c r="L13" s="10"/>
     </row>
     <row r="14" spans="2:18" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="59" t="s">
-        <v>68</v>
-      </c>
-      <c r="D14" s="15" t="s">
+      <c r="B14" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" s="57" t="s">
         <v>40</v>
       </c>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="17"/>
+      <c r="E14" s="58"/>
+      <c r="F14" s="58"/>
+      <c r="G14" s="59"/>
       <c r="H14" s="10"/>
-      <c r="I14" s="21" t="s">
+      <c r="I14" s="63" t="s">
         <v>41</v>
       </c>
-      <c r="J14" s="22"/>
-      <c r="K14" s="22"/>
-      <c r="L14" s="23"/>
+      <c r="J14" s="64"/>
+      <c r="K14" s="64"/>
+      <c r="L14" s="65"/>
     </row>
     <row r="15" spans="2:18" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D15" s="10"/>
@@ -2246,122 +2304,118 @@
       <c r="L15" s="10"/>
     </row>
     <row r="16" spans="2:18" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="60" t="s">
+      <c r="B16" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="D16" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" s="49"/>
+      <c r="F16" s="49"/>
+      <c r="G16" s="50"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="51" t="s">
+        <v>43</v>
+      </c>
+      <c r="J16" s="52"/>
+      <c r="K16" s="52"/>
+      <c r="L16" s="53"/>
+    </row>
+    <row r="17" spans="2:12" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="38"/>
+      <c r="I17" s="38"/>
+      <c r="J17" s="38"/>
+      <c r="K17" s="38"/>
+      <c r="L17" s="38"/>
+    </row>
+    <row r="18" spans="2:12" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="D18" s="54" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18" s="55"/>
+      <c r="F18" s="55"/>
+      <c r="G18" s="55"/>
+      <c r="H18" s="55"/>
+      <c r="I18" s="55"/>
+      <c r="J18" s="55"/>
+      <c r="K18" s="55"/>
+      <c r="L18" s="56"/>
+    </row>
+    <row r="19" spans="2:12" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D19" s="38"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="38"/>
+      <c r="I19" s="38"/>
+      <c r="J19" s="38"/>
+      <c r="K19" s="38"/>
+      <c r="L19" s="38"/>
+    </row>
+    <row r="20" spans="2:12" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="D16" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="J16" s="28"/>
-      <c r="K16" s="28"/>
-      <c r="L16" s="29"/>
-    </row>
-    <row r="17" spans="2:12" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="30"/>
-      <c r="G17" s="30"/>
-      <c r="H17" s="30"/>
-      <c r="I17" s="30"/>
-      <c r="J17" s="30"/>
-      <c r="K17" s="30"/>
-      <c r="L17" s="30"/>
-    </row>
-    <row r="18" spans="2:12" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="61" t="s">
-        <v>61</v>
-      </c>
-      <c r="D18" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="E18" s="32"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="32"/>
-      <c r="H18" s="32"/>
-      <c r="I18" s="32"/>
-      <c r="J18" s="32"/>
-      <c r="K18" s="32"/>
-      <c r="L18" s="33"/>
-    </row>
-    <row r="19" spans="2:12" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D19" s="30"/>
-      <c r="E19" s="30"/>
-      <c r="F19" s="30"/>
-      <c r="G19" s="30"/>
-      <c r="H19" s="30"/>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
-      <c r="K19" s="30"/>
-      <c r="L19" s="30"/>
-    </row>
-    <row r="20" spans="2:12" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="62" t="s">
-        <v>62</v>
-      </c>
-      <c r="D20" s="37" t="s">
-        <v>53</v>
-      </c>
-      <c r="E20" s="38"/>
-      <c r="F20" s="38"/>
-      <c r="G20" s="38"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="38"/>
-      <c r="J20" s="38"/>
-      <c r="K20" s="38"/>
-      <c r="L20" s="39"/>
+      <c r="D20" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="E20" s="40"/>
+      <c r="F20" s="40"/>
+      <c r="G20" s="40"/>
+      <c r="H20" s="40"/>
+      <c r="I20" s="40"/>
+      <c r="J20" s="40"/>
+      <c r="K20" s="40"/>
+      <c r="L20" s="41"/>
     </row>
     <row r="21" spans="2:12" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D21" s="30"/>
-      <c r="E21" s="30"/>
-      <c r="F21" s="30"/>
-      <c r="G21" s="30"/>
-      <c r="H21" s="30"/>
-      <c r="I21" s="30"/>
-      <c r="J21" s="30"/>
-      <c r="K21" s="30"/>
-      <c r="L21" s="30"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="38"/>
+      <c r="H21" s="38"/>
+      <c r="I21" s="38"/>
+      <c r="J21" s="38"/>
+      <c r="K21" s="38"/>
+      <c r="L21" s="38"/>
     </row>
     <row r="22" spans="2:12" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="63" t="s">
-        <v>63</v>
-      </c>
-      <c r="D22" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="E22" s="35"/>
-      <c r="F22" s="35"/>
-      <c r="G22" s="35"/>
-      <c r="H22" s="35"/>
-      <c r="I22" s="35"/>
-      <c r="J22" s="35"/>
-      <c r="K22" s="35"/>
-      <c r="L22" s="36"/>
+      <c r="B22" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="D22" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="E22" s="36"/>
+      <c r="F22" s="36"/>
+      <c r="G22" s="36"/>
+      <c r="H22" s="36"/>
+      <c r="I22" s="36"/>
+      <c r="J22" s="36"/>
+      <c r="K22" s="36"/>
+      <c r="L22" s="37"/>
     </row>
     <row r="23" spans="2:12" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="D23" s="30"/>
-      <c r="E23" s="30"/>
-      <c r="F23" s="30"/>
-      <c r="G23" s="30"/>
-      <c r="H23" s="30"/>
-      <c r="I23" s="30"/>
-      <c r="J23" s="30"/>
-      <c r="K23" s="30"/>
-      <c r="L23" s="30"/>
+      <c r="D23" s="38"/>
+      <c r="E23" s="38"/>
+      <c r="F23" s="38"/>
+      <c r="G23" s="38"/>
+      <c r="H23" s="38"/>
+      <c r="I23" s="38"/>
+      <c r="J23" s="38"/>
+      <c r="K23" s="38"/>
+      <c r="L23" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="D2:L2"/>
-    <mergeCell ref="D5:L5"/>
-    <mergeCell ref="D6:L6"/>
-    <mergeCell ref="D7:L7"/>
-    <mergeCell ref="D8:L8"/>
+    <mergeCell ref="D9:L9"/>
     <mergeCell ref="D22:L22"/>
     <mergeCell ref="D23:L23"/>
     <mergeCell ref="D20:L20"/>
@@ -2375,9 +2429,13 @@
     <mergeCell ref="D18:L18"/>
     <mergeCell ref="D21:L21"/>
     <mergeCell ref="D14:G14"/>
+    <mergeCell ref="I14:L14"/>
+    <mergeCell ref="D2:L2"/>
+    <mergeCell ref="D5:L5"/>
+    <mergeCell ref="D6:L6"/>
+    <mergeCell ref="D7:L7"/>
+    <mergeCell ref="D8:L8"/>
     <mergeCell ref="D4:L4"/>
-    <mergeCell ref="I14:L14"/>
-    <mergeCell ref="D9:L9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
création des dlg au menu principal
</commit_message>
<xml_diff>
--- a/docs/data.xlsx
+++ b/docs/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\XD5965\Creative Cloud Files\01_PROJETS\01_PROG\01_APP\MyDLG\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Creative Cloud Files\01_PROJETS\01_PROG\01_APP\MyDLG\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4673F1C0-2BBE-48A4-B87A-47DFEBD7CBEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDEA474A-7C26-423F-86E6-02E5FDFE774F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8D14DDDC-9FC9-425C-962E-B3AF6E914BB2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{8D14DDDC-9FC9-425C-962E-B3AF6E914BB2}"/>
   </bookViews>
   <sheets>
     <sheet name="Tables" sheetId="1" r:id="rId1"/>
@@ -1098,7 +1098,43 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1183,42 +1219,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1551,7 +1551,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFC023DF-5960-4085-8D7D-5FF8A6FE382A}">
   <dimension ref="B2:O35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
@@ -2073,8 +2073,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24577A07-6CE2-46BC-965D-BF8C33E092FF}">
   <dimension ref="B1:R23"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:L22"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -2097,17 +2097,17 @@
       <c r="B2" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="D2" s="55" t="s">
+      <c r="D2" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="56"/>
-      <c r="J2" s="56"/>
-      <c r="K2" s="56"/>
-      <c r="L2" s="57"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="28"/>
     </row>
     <row r="3" spans="2:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D3" s="9"/>
@@ -2124,101 +2124,101 @@
       <c r="B4" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="D4" s="64" t="s">
+      <c r="D4" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="E4" s="65"/>
-      <c r="F4" s="65"/>
-      <c r="G4" s="65"/>
-      <c r="H4" s="65"/>
-      <c r="I4" s="65"/>
-      <c r="J4" s="65"/>
-      <c r="K4" s="65"/>
-      <c r="L4" s="66"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="37"/>
+      <c r="K4" s="37"/>
+      <c r="L4" s="38"/>
     </row>
     <row r="5" spans="2:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="26"/>
-      <c r="K5" s="26"/>
-      <c r="L5" s="26"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="29"/>
+      <c r="L5" s="29"/>
     </row>
     <row r="6" spans="2:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="D6" s="58" t="s">
+      <c r="D6" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="59"/>
-      <c r="F6" s="59"/>
-      <c r="G6" s="59"/>
-      <c r="H6" s="59"/>
-      <c r="I6" s="59"/>
-      <c r="J6" s="59"/>
-      <c r="K6" s="59"/>
-      <c r="L6" s="60"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="31"/>
+      <c r="J6" s="31"/>
+      <c r="K6" s="31"/>
+      <c r="L6" s="32"/>
     </row>
     <row r="7" spans="2:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="26"/>
-      <c r="J7" s="26"/>
-      <c r="K7" s="26"/>
-      <c r="L7" s="26"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="29"/>
+      <c r="I7" s="29"/>
+      <c r="J7" s="29"/>
+      <c r="K7" s="29"/>
+      <c r="L7" s="29"/>
     </row>
     <row r="8" spans="2:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="D8" s="61" t="s">
+      <c r="D8" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="E8" s="62"/>
-      <c r="F8" s="62"/>
-      <c r="G8" s="62"/>
-      <c r="H8" s="62"/>
-      <c r="I8" s="62"/>
-      <c r="J8" s="62"/>
-      <c r="K8" s="62"/>
-      <c r="L8" s="63"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="34"/>
+      <c r="I8" s="34"/>
+      <c r="J8" s="34"/>
+      <c r="K8" s="34"/>
+      <c r="L8" s="35"/>
       <c r="P8" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="9" spans="2:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="26"/>
-      <c r="J9" s="26"/>
-      <c r="K9" s="26"/>
-      <c r="L9" s="26"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="29"/>
+      <c r="K9" s="29"/>
+      <c r="L9" s="29"/>
     </row>
     <row r="10" spans="2:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="D10" s="34" t="s">
+      <c r="D10" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="35"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="35"/>
-      <c r="H10" s="35"/>
-      <c r="I10" s="35"/>
-      <c r="J10" s="35"/>
-      <c r="K10" s="35"/>
-      <c r="L10" s="36"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="47"/>
+      <c r="H10" s="47"/>
+      <c r="I10" s="47"/>
+      <c r="J10" s="47"/>
+      <c r="K10" s="47"/>
+      <c r="L10" s="48"/>
       <c r="P10" s="1" t="s">
         <v>45</v>
       </c>
@@ -2230,15 +2230,15 @@
       </c>
     </row>
     <row r="11" spans="2:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D11" s="30"/>
-      <c r="E11" s="30"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="30"/>
-      <c r="H11" s="30"/>
-      <c r="I11" s="30"/>
-      <c r="J11" s="30"/>
-      <c r="K11" s="30"/>
-      <c r="L11" s="30"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="42"/>
+      <c r="J11" s="42"/>
+      <c r="K11" s="42"/>
+      <c r="L11" s="42"/>
       <c r="P11" s="1" t="s">
         <v>49</v>
       </c>
@@ -2253,17 +2253,17 @@
       <c r="B12" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="D12" s="37" t="s">
+      <c r="D12" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="38"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="38"/>
-      <c r="J12" s="38"/>
-      <c r="K12" s="38"/>
-      <c r="L12" s="39"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="50"/>
+      <c r="H12" s="50"/>
+      <c r="I12" s="50"/>
+      <c r="J12" s="50"/>
+      <c r="K12" s="50"/>
+      <c r="L12" s="51"/>
     </row>
     <row r="13" spans="2:18" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D13" s="10"/>
@@ -2280,19 +2280,19 @@
       <c r="B14" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="D14" s="49" t="s">
+      <c r="D14" s="61" t="s">
         <v>40</v>
       </c>
-      <c r="E14" s="50"/>
-      <c r="F14" s="50"/>
-      <c r="G14" s="51"/>
+      <c r="E14" s="62"/>
+      <c r="F14" s="62"/>
+      <c r="G14" s="63"/>
       <c r="H14" s="10"/>
-      <c r="I14" s="52" t="s">
+      <c r="I14" s="64" t="s">
         <v>41</v>
       </c>
-      <c r="J14" s="53"/>
-      <c r="K14" s="53"/>
-      <c r="L14" s="54"/>
+      <c r="J14" s="65"/>
+      <c r="K14" s="65"/>
+      <c r="L14" s="66"/>
     </row>
     <row r="15" spans="2:18" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D15" s="10"/>
@@ -2309,120 +2309,123 @@
       <c r="B16" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="D16" s="40" t="s">
+      <c r="D16" s="52" t="s">
         <v>42</v>
       </c>
-      <c r="E16" s="41"/>
-      <c r="F16" s="41"/>
-      <c r="G16" s="42"/>
+      <c r="E16" s="53"/>
+      <c r="F16" s="53"/>
+      <c r="G16" s="54"/>
       <c r="H16" s="10"/>
-      <c r="I16" s="43" t="s">
+      <c r="I16" s="55" t="s">
         <v>43</v>
       </c>
-      <c r="J16" s="44"/>
-      <c r="K16" s="44"/>
-      <c r="L16" s="45"/>
-    </row>
-    <row r="17" spans="2:12" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="30"/>
-      <c r="G17" s="30"/>
-      <c r="H17" s="30"/>
-      <c r="I17" s="30"/>
-      <c r="J17" s="30"/>
-      <c r="K17" s="30"/>
-      <c r="L17" s="30"/>
-    </row>
-    <row r="18" spans="2:12" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J16" s="56"/>
+      <c r="K16" s="56"/>
+      <c r="L16" s="57"/>
+    </row>
+    <row r="17" spans="2:13" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="42"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
+      <c r="K17" s="42"/>
+      <c r="L17" s="42"/>
+    </row>
+    <row r="18" spans="2:13" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="D18" s="46" t="s">
+      <c r="D18" s="58" t="s">
         <v>44</v>
       </c>
-      <c r="E18" s="47"/>
-      <c r="F18" s="47"/>
-      <c r="G18" s="47"/>
-      <c r="H18" s="47"/>
-      <c r="I18" s="47"/>
-      <c r="J18" s="47"/>
-      <c r="K18" s="47"/>
-      <c r="L18" s="48"/>
-    </row>
-    <row r="19" spans="2:12" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D19" s="30"/>
-      <c r="E19" s="30"/>
-      <c r="F19" s="30"/>
-      <c r="G19" s="30"/>
-      <c r="H19" s="30"/>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
-      <c r="K19" s="30"/>
-      <c r="L19" s="30"/>
-    </row>
-    <row r="20" spans="2:12" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E18" s="59"/>
+      <c r="F18" s="59"/>
+      <c r="G18" s="59"/>
+      <c r="H18" s="59"/>
+      <c r="I18" s="59"/>
+      <c r="J18" s="59"/>
+      <c r="K18" s="59"/>
+      <c r="L18" s="60"/>
+      <c r="M18" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D19" s="42"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="42"/>
+      <c r="G19" s="42"/>
+      <c r="H19" s="42"/>
+      <c r="I19" s="42"/>
+      <c r="J19" s="42"/>
+      <c r="K19" s="42"/>
+      <c r="L19" s="42"/>
+    </row>
+    <row r="20" spans="2:13" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="D20" s="31" t="s">
+      <c r="D20" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="E20" s="32"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="32"/>
-      <c r="H20" s="32"/>
-      <c r="I20" s="32"/>
-      <c r="J20" s="32"/>
-      <c r="K20" s="32"/>
-      <c r="L20" s="33"/>
-    </row>
-    <row r="21" spans="2:12" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D21" s="30"/>
-      <c r="E21" s="30"/>
-      <c r="F21" s="30"/>
-      <c r="G21" s="30"/>
-      <c r="H21" s="30"/>
-      <c r="I21" s="30"/>
-      <c r="J21" s="30"/>
-      <c r="K21" s="30"/>
-      <c r="L21" s="30"/>
-    </row>
-    <row r="22" spans="2:12" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E20" s="44"/>
+      <c r="F20" s="44"/>
+      <c r="G20" s="44"/>
+      <c r="H20" s="44"/>
+      <c r="I20" s="44"/>
+      <c r="J20" s="44"/>
+      <c r="K20" s="44"/>
+      <c r="L20" s="45"/>
+      <c r="M20" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D21" s="42"/>
+      <c r="E21" s="42"/>
+      <c r="F21" s="42"/>
+      <c r="G21" s="42"/>
+      <c r="H21" s="42"/>
+      <c r="I21" s="42"/>
+      <c r="J21" s="42"/>
+      <c r="K21" s="42"/>
+      <c r="L21" s="42"/>
+    </row>
+    <row r="22" spans="2:13" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="D22" s="27" t="s">
+      <c r="D22" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="28"/>
-      <c r="H22" s="28"/>
-      <c r="I22" s="28"/>
-      <c r="J22" s="28"/>
-      <c r="K22" s="28"/>
-      <c r="L22" s="29"/>
-    </row>
-    <row r="23" spans="2:12" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="D23" s="30"/>
-      <c r="E23" s="30"/>
-      <c r="F23" s="30"/>
-      <c r="G23" s="30"/>
-      <c r="H23" s="30"/>
-      <c r="I23" s="30"/>
-      <c r="J23" s="30"/>
-      <c r="K23" s="30"/>
-      <c r="L23" s="30"/>
+      <c r="E22" s="40"/>
+      <c r="F22" s="40"/>
+      <c r="G22" s="40"/>
+      <c r="H22" s="40"/>
+      <c r="I22" s="40"/>
+      <c r="J22" s="40"/>
+      <c r="K22" s="40"/>
+      <c r="L22" s="41"/>
+      <c r="M22" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="D23" s="42"/>
+      <c r="E23" s="42"/>
+      <c r="F23" s="42"/>
+      <c r="G23" s="42"/>
+      <c r="H23" s="42"/>
+      <c r="I23" s="42"/>
+      <c r="J23" s="42"/>
+      <c r="K23" s="42"/>
+      <c r="L23" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="D2:L2"/>
-    <mergeCell ref="D5:L5"/>
-    <mergeCell ref="D6:L6"/>
-    <mergeCell ref="D7:L7"/>
-    <mergeCell ref="D8:L8"/>
-    <mergeCell ref="D4:L4"/>
     <mergeCell ref="D9:L9"/>
     <mergeCell ref="D22:L22"/>
     <mergeCell ref="D23:L23"/>
@@ -2438,6 +2441,12 @@
     <mergeCell ref="D21:L21"/>
     <mergeCell ref="D14:G14"/>
     <mergeCell ref="I14:L14"/>
+    <mergeCell ref="D2:L2"/>
+    <mergeCell ref="D5:L5"/>
+    <mergeCell ref="D6:L6"/>
+    <mergeCell ref="D7:L7"/>
+    <mergeCell ref="D8:L8"/>
+    <mergeCell ref="D4:L4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>